<commit_message>
PCBs: update of validation results of CC1101_868MHz_RF_Modul_FUEL4EP and CC1101_868MHz_UFL_RF_Modul_FUEL4EP: added RSSI sensitivities
</commit_message>
<xml_diff>
--- a/AsksinPP_developments/PCBs/CC1101_868MHz_RF_Modul_FUEL4EP/Prototype_Validation/validation_results.xlsx
+++ b/AsksinPP_developments/PCBs/CC1101_868MHz_RF_Modul_FUEL4EP/Prototype_Validation/validation_results.xlsx
@@ -20,7 +20,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="33">
+  <si>
+    <t xml:space="preserve">1. Frequenzmessung am GD0 Pin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frequenzmessung mit Rigol DG1022Z Frequenzzähler mit hochgenauem externen 10 MHz Referenztakt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 MHz Referenztakt mit Mini Precision GPS Reference Clock Modul von Leo Bodnar</t>
+  </si>
   <si>
     <t xml:space="preserve">#Index</t>
   </si>
@@ -91,6 +100,38 @@
   </si>
   <si>
     <t xml:space="preserve">eByte E07-868MS10 10019-V1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. RSSI Empfangspegel mit Frequenztest mit ‚Active Ping’</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gemessen mit Frequenztest mit ‚active Ping’: RSSI Wert des Signals von der Zentrale  bei 868,3 MHz, siehe FreqTest_active_ping_serial_monitor_&lt;#index&gt;.log</t>
+  </si>
+  <si>
+    <t xml:space="preserve">die Module unter Test (Device under Test DUT) wurden an der gleichen Stelle im Wohnzimmer mit dem identischen Frequenztest-Skript vermessen. Die Zentrale ist zwei Stockwerke höher im Dachgeschoss. Dazwischen sind 2 Betondecken.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RSSI Pegel
+[dBm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wertung
+(1 = beste)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Antennentyp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Draht</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uFL Stabantenne</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eByte E07-900MM10S </t>
   </si>
 </sst>
 </file>
@@ -102,7 +143,7 @@
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -124,6 +165,19 @@
       <family val="0"/>
     </font>
     <font>
+      <b val="true"/>
+      <sz val="14"/>
+      <color rgb="FF3465A4"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="8"/>
       <name val="FreeSans"/>
       <family val="2"/>
@@ -139,7 +193,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -149,13 +203,37 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00A933"/>
-        <bgColor rgb="FF008000"/>
+        <bgColor rgb="FF069A2E"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF8000"/>
-        <bgColor rgb="FFFF6600"/>
+        <bgColor rgb="FFFF5429"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF77BC65"/>
+        <bgColor rgb="FF99CC00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF069A2E"/>
+        <bgColor rgb="FF00A933"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFFF5429"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF5429"/>
+        <bgColor rgb="FFFF8000"/>
       </patternFill>
     </fill>
   </fills>
@@ -200,7 +278,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="26">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -209,10 +287,42 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -221,15 +331,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -245,16 +351,36 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -277,7 +403,7 @@
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF069A2E"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
@@ -313,9 +439,9 @@
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF8000"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FFFF5429"/>
+      <rgbColor rgb="FF3465A4"/>
+      <rgbColor rgb="FF77BC65"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF00A933"/>
       <rgbColor rgb="FF003300"/>
@@ -334,10 +460,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:O26"/>
+  <dimension ref="A1:O34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I24" activeCellId="0" sqref="I24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -359,356 +485,540 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="31.3"/>
   </cols>
   <sheetData>
-    <row r="1" s="5" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="5" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="0"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+    </row>
+    <row r="2" s="5" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="0"/>
+      <c r="E2" s="0"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+    </row>
+    <row r="3" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+    </row>
+    <row r="4" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+    </row>
+    <row r="5" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+    </row>
+    <row r="6" s="5" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="B6" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="C6" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="D6" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="E6" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="F6" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="G6" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="H6" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="I6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="J6" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="K6" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="L6" s="11" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" s="5" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="n">
+      <c r="M6" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="N6" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="O6" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" s="5" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="7" t="n">
+      <c r="B7" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="14" t="n">
         <v>10</v>
       </c>
-      <c r="D2" s="7" t="n">
+      <c r="D7" s="14" t="n">
         <v>10</v>
       </c>
-      <c r="E2" s="2" t="n">
+      <c r="E7" s="9" t="n">
         <v>135417.746617</v>
       </c>
-      <c r="F2" s="2" t="n">
+      <c r="F7" s="9" t="n">
         <v>537</v>
       </c>
-      <c r="G2" s="2" t="n">
+      <c r="G7" s="9" t="n">
         <v>135417.746591</v>
       </c>
-      <c r="H2" s="2" t="n">
+      <c r="H7" s="9" t="n">
         <v>135417.744826</v>
       </c>
-      <c r="I2" s="2" t="n">
+      <c r="I7" s="9" t="n">
         <v>26000000</v>
       </c>
-      <c r="J2" s="2" t="n">
+      <c r="J7" s="9" t="n">
         <v>192</v>
       </c>
-      <c r="K2" s="2" t="n">
-        <f aca="false">I2/J2</f>
+      <c r="K7" s="9" t="n">
+        <f aca="false">I7/J7</f>
         <v>135416.666666667</v>
       </c>
-      <c r="L2" s="8" t="n">
-        <f aca="false">(E2-K2)/K2*1000000</f>
+      <c r="L7" s="15" t="n">
+        <f aca="false">(E7-K7)/K7*1000000</f>
         <v>7.9750178436247</v>
       </c>
-      <c r="M2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="O2" s="9" t="n">
-        <f aca="false">F2/K2</f>
+      <c r="M7" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="N7" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="O7" s="16" t="n">
+        <f aca="false">F7/K7</f>
         <v>0.00396553846153846</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="10" t="n">
+    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="10" t="n">
+      <c r="B8" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="17" t="n">
         <v>10</v>
       </c>
-      <c r="D3" s="10" t="n">
+      <c r="D8" s="17" t="n">
         <v>10</v>
       </c>
-      <c r="E3" s="10" t="n">
+      <c r="E8" s="17" t="n">
         <v>135417.925391</v>
       </c>
-      <c r="F3" s="10" t="n">
+      <c r="F8" s="17" t="n">
         <v>19090</v>
       </c>
-      <c r="G3" s="10" t="n">
+      <c r="G8" s="17" t="n">
         <v>135417.890165</v>
       </c>
-      <c r="H3" s="10" t="n">
+      <c r="H8" s="17" t="n">
         <v>135417.952587</v>
       </c>
-      <c r="I3" s="2" t="n">
+      <c r="I8" s="9" t="n">
         <v>26000000</v>
       </c>
-      <c r="J3" s="2" t="n">
+      <c r="J8" s="9" t="n">
         <v>192</v>
       </c>
-      <c r="K3" s="2" t="n">
-        <f aca="false">I3/J3</f>
+      <c r="K8" s="9" t="n">
+        <f aca="false">I8/J8</f>
         <v>135416.666666667</v>
       </c>
-      <c r="L3" s="8" t="n">
-        <f aca="false">(E3-K3)/K3*1000000</f>
+      <c r="L8" s="15" t="n">
+        <f aca="false">(E8-K8)/K8*1000000</f>
         <v>9.29519507439375</v>
       </c>
-      <c r="M3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="O3" s="9" t="n">
-        <f aca="false">F3/K3</f>
+      <c r="M8" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="N8" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="O8" s="16" t="n">
+        <f aca="false">F8/K8</f>
         <v>0.140972307692308</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="10" t="n">
+    <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="17" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="10" t="n">
+      <c r="B9" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="17" t="n">
         <v>10</v>
       </c>
-      <c r="D4" s="10" t="n">
+      <c r="D9" s="17" t="n">
         <v>10</v>
       </c>
-      <c r="E4" s="10" t="n">
+      <c r="E9" s="17" t="n">
         <v>135417.503672</v>
       </c>
-      <c r="F4" s="10" t="n">
+      <c r="F9" s="17" t="n">
         <v>11639</v>
       </c>
-      <c r="G4" s="10" t="n">
+      <c r="G9" s="17" t="n">
         <v>135417.484026</v>
       </c>
-      <c r="H4" s="10" t="n">
+      <c r="H9" s="17" t="n">
         <v>135417.522114</v>
       </c>
-      <c r="I4" s="2" t="n">
+      <c r="I9" s="9" t="n">
         <v>26000000</v>
       </c>
-      <c r="J4" s="2" t="n">
+      <c r="J9" s="9" t="n">
         <v>192</v>
       </c>
-      <c r="K4" s="2" t="n">
-        <f aca="false">I4/J4</f>
+      <c r="K9" s="9" t="n">
+        <f aca="false">I9/J9</f>
         <v>135416.666666667</v>
       </c>
-      <c r="L4" s="8" t="n">
-        <f aca="false">(E4-K4)/K4*1000000</f>
+      <c r="L9" s="15" t="n">
+        <f aca="false">(E9-K9)/K9*1000000</f>
         <v>6.18096245896929</v>
       </c>
-      <c r="M4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="O4" s="9" t="n">
-        <f aca="false">F4/K4</f>
+      <c r="M9" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="N9" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="O9" s="16" t="n">
+        <f aca="false">F9/K9</f>
         <v>0.0859495384615385</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="10" t="n">
+    <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="17" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="10" t="n">
+      <c r="B10" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="17" t="n">
         <v>10</v>
       </c>
-      <c r="D5" s="10" t="n">
+      <c r="D10" s="17" t="n">
         <v>10</v>
       </c>
-      <c r="E5" s="10" t="n">
+      <c r="E10" s="17" t="n">
         <v>135417.791406</v>
       </c>
-      <c r="F5" s="10" t="n">
+      <c r="F10" s="17" t="n">
         <v>9308</v>
       </c>
-      <c r="G5" s="10" t="n">
+      <c r="G10" s="17" t="n">
         <v>135417.774899</v>
       </c>
-      <c r="H5" s="10" t="n">
+      <c r="H10" s="17" t="n">
         <v>135417.808699</v>
       </c>
-      <c r="I5" s="2" t="n">
+      <c r="I10" s="9" t="n">
         <v>26000000</v>
       </c>
-      <c r="J5" s="2" t="n">
+      <c r="J10" s="9" t="n">
         <v>192</v>
       </c>
-      <c r="K5" s="2" t="n">
-        <f aca="false">I5/J5</f>
+      <c r="K10" s="9" t="n">
+        <f aca="false">I10/J10</f>
         <v>135416.666666667</v>
       </c>
-      <c r="L5" s="8" t="n">
-        <f aca="false">(E5-K5)/K5*1000000</f>
+      <c r="L10" s="15" t="n">
+        <f aca="false">(E10-K10)/K10*1000000</f>
         <v>8.30576738213688</v>
       </c>
-      <c r="M5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="N5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="O5" s="9" t="n">
-        <f aca="false">F5/K5</f>
+      <c r="M10" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="N10" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="O10" s="16" t="n">
+        <f aca="false">F10/K10</f>
         <v>0.068736</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="10" t="n">
+    <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="17" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B11" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="17" t="n">
+        <v>10</v>
+      </c>
+      <c r="D11" s="17" t="n">
+        <v>10</v>
+      </c>
+      <c r="E11" s="17" t="n">
+        <v>135414.913377</v>
+      </c>
+      <c r="F11" s="17" t="n">
+        <v>705</v>
+      </c>
+      <c r="G11" s="17" t="n">
+        <v>135414.912082</v>
+      </c>
+      <c r="H11" s="17" t="n">
+        <v>135414.914604</v>
+      </c>
+      <c r="I11" s="9" t="n">
+        <v>26000000</v>
+      </c>
+      <c r="J11" s="9" t="n">
+        <v>192</v>
+      </c>
+      <c r="K11" s="9" t="n">
+        <f aca="false">I11/J11</f>
+        <v>135416.666666667</v>
+      </c>
+      <c r="L11" s="20" t="n">
+        <f aca="false">(E11-K11)/K11*1000000</f>
+        <v>-12.9473698487362</v>
+      </c>
+      <c r="M11" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="10" t="n">
-        <v>10</v>
-      </c>
-      <c r="D6" s="10" t="n">
-        <v>10</v>
-      </c>
-      <c r="E6" s="10" t="n">
-        <v>135414.913377</v>
-      </c>
-      <c r="F6" s="10" t="n">
-        <v>705</v>
-      </c>
-      <c r="G6" s="10" t="n">
-        <v>135414.912082</v>
-      </c>
-      <c r="H6" s="10" t="n">
-        <v>135414.914604</v>
-      </c>
-      <c r="I6" s="2" t="n">
-        <v>26000000</v>
-      </c>
-      <c r="J6" s="2" t="n">
-        <v>192</v>
-      </c>
-      <c r="K6" s="2" t="n">
-        <f aca="false">I6/J6</f>
-        <v>135416.666666667</v>
-      </c>
-      <c r="L6" s="13" t="n">
-        <f aca="false">(E6-K6)/K6*1000000</f>
-        <v>-12.9473698487362</v>
-      </c>
-      <c r="M6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="N6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="O6" s="9" t="n">
-        <f aca="false">F6/K6</f>
+      <c r="N11" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="O11" s="16" t="n">
+        <f aca="false">F11/K11</f>
         <v>0.00520615384615385</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1"/>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1"/>
+    <row r="13" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="0"/>
+    </row>
+    <row r="14" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1"/>
+      <c r="A15" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1"/>
+      <c r="A16" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1"/>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1"/>
+    <row r="18" customFormat="false" ht="24.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1"/>
+      <c r="A19" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="17" t="n">
+        <v>-56</v>
+      </c>
+      <c r="D19" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="E19" s="17" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1"/>
+      <c r="A20" s="17" t="n">
+        <v>2</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1"/>
+      <c r="A21" s="17" t="n">
+        <v>3</v>
+      </c>
+      <c r="B21" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="17" t="n">
+        <v>-58</v>
+      </c>
+      <c r="D21" s="23" t="n">
+        <v>2</v>
+      </c>
+      <c r="E21" s="17" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1"/>
+      <c r="A22" s="17" t="n">
+        <v>4</v>
+      </c>
+      <c r="B22" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1"/>
+      <c r="A23" s="17" t="n">
+        <v>5</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="17" t="n">
+        <v>-66</v>
+      </c>
+      <c r="D23" s="24" t="n">
+        <v>4</v>
+      </c>
+      <c r="E23" s="17" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1"/>
+      <c r="A24" s="17" t="n">
+        <v>6</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="17" t="n">
+        <v>-60</v>
+      </c>
+      <c r="D24" s="25" t="n">
+        <v>3</v>
+      </c>
+      <c r="E24" s="17" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1"/>
@@ -716,7 +1026,34 @@
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1"/>
     </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
PCBs: update of validation results of CC1101_868MHz_RF_Modul_FUEL4EP and CC1101_868MHz_UFL_RF_Modul_FUEL4EP
</commit_message>
<xml_diff>
--- a/AsksinPP_developments/PCBs/CC1101_868MHz_RF_Modul_FUEL4EP/Prototype_Validation/validation_results.xlsx
+++ b/AsksinPP_developments/PCBs/CC1101_868MHz_RF_Modul_FUEL4EP/Prototype_Validation/validation_results.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="38">
   <si>
     <t xml:space="preserve">1. Frequenzmessung am GD0 Pin</t>
   </si>
@@ -105,10 +105,16 @@
     <t xml:space="preserve">2. RSSI Empfangspegel mit Frequenztest mit ‚Active Ping’</t>
   </si>
   <si>
-    <t xml:space="preserve">gemessen mit Frequenztest mit ‚active Ping’: RSSI Wert des Signals von der Zentrale  bei 868,3 MHz, siehe FreqTest_active_ping_serial_monitor_&lt;#index&gt;.log</t>
-  </si>
-  <si>
-    <t xml:space="preserve">die Module unter Test (Device under Test DUT) wurden an der gleichen Stelle im Wohnzimmer mit dem identischen Frequenztest-Skript vermessen. Die Zentrale ist zwei Stockwerke höher im Dachgeschoss. Dazwischen sind 2 Betondecken.  </t>
+    <t xml:space="preserve">Die gemessenen RSSI Werte sind nur als grobe Indikation des Empfangspegels zu sehen. Sie schwanken in aufeinanderfolgenden Messungen und hängen auch von kleinen Veränderungen, z.B. Bewegungen, im Umfeld ab.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a) mit zwei Betondecken zwischen  Zentrale und Empfänger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gemessen mit Frequenztest mit ‚active Ping’: RSSI Wert des Signals von der Zentrale  bei 868,3 MHz, siehe FreqTest_active_ping_serial_monitor_&lt;#index&gt;_Erdgeschoss.log</t>
+  </si>
+  <si>
+    <t xml:space="preserve">die Module unter Test (Device under Test DUT) wurden an der gleichen Stelle im Erdgeschoß mit dem identischen Frequenztest-Skript vermessen. Die Zentrale ist zwei Stockwerke höher im Dachgeschoss. Dazwischen sind 2 Betondecken.  </t>
   </si>
   <si>
     <t xml:space="preserve">RSSI Pegel
@@ -132,6 +138,15 @@
   </si>
   <si>
     <t xml:space="preserve">eByte E07-900MM10S </t>
+  </si>
+  <si>
+    <t xml:space="preserve">b) mit drei Betondecken zwischen  Zentrale und Empfänger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gemessen mit Frequenztest mit ‚active Ping’: RSSI Wert des Signals von der Zentrale  bei 868,3 MHz, siehe FreqTest_active_ping_serial_monitor_&lt;#index&gt;_Keller.log</t>
+  </si>
+  <si>
+    <t xml:space="preserve">die Module unter Test (Device under Test DUT) wurden an der gleichen Stelle im Keller  mit dem identischen Frequenztest-Skript vermessen. Die Zentrale ist drei  Stockwerke höher im Dachgeschoss. Dazwischen sind 3 Betondecken.  </t>
   </si>
 </sst>
 </file>
@@ -278,7 +293,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -363,6 +378,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -380,6 +399,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -460,10 +483,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:O34"/>
+  <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I22" activeCellId="0" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -891,164 +914,299 @@
       <c r="D14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="21" t="s">
         <v>24</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="0"/>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="6" t="s">
-        <v>25</v>
-      </c>
+    <row r="16" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="0"/>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1"/>
-    </row>
-    <row r="18" customFormat="false" ht="24.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="9" t="s">
+    <row r="17" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="0"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="0"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="0"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1"/>
+    </row>
+    <row r="21" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B21" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="D18" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="E18" s="17" t="s">
+      <c r="C21" s="11" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="9" t="n">
+      <c r="D21" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21" s="17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="B22" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="17" t="n">
+      <c r="C22" s="17" t="n">
         <v>-56</v>
       </c>
-      <c r="D19" s="22" t="n">
+      <c r="D22" s="23" t="n">
         <v>1</v>
       </c>
-      <c r="E19" s="17" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="17" t="n">
-        <v>2</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="17" t="n">
-        <v>3</v>
-      </c>
-      <c r="B21" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" s="17" t="n">
-        <v>-58</v>
-      </c>
-      <c r="D21" s="23" t="n">
-        <v>2</v>
-      </c>
-      <c r="E21" s="17" t="s">
+      <c r="E22" s="17" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="17" t="n">
-        <v>4</v>
-      </c>
-      <c r="B22" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="17" t="n">
-        <v>5</v>
-      </c>
-      <c r="B23" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="C23" s="17" t="n">
-        <v>-66</v>
-      </c>
-      <c r="D23" s="24" t="n">
-        <v>4</v>
-      </c>
-      <c r="E23" s="17" t="s">
-        <v>29</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="17" t="n">
+        <v>3</v>
+      </c>
+      <c r="B24" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" s="17" t="n">
+        <v>-58</v>
+      </c>
+      <c r="D24" s="24" t="n">
+        <v>2</v>
+      </c>
+      <c r="E24" s="17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="17" t="n">
+        <v>4</v>
+      </c>
+      <c r="B25" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="17" t="n">
+        <v>5</v>
+      </c>
+      <c r="B26" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" s="17" t="n">
+        <v>-66</v>
+      </c>
+      <c r="D26" s="25" t="n">
+        <v>4</v>
+      </c>
+      <c r="E26" s="17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="17" t="n">
         <v>6</v>
       </c>
-      <c r="B24" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="C24" s="17" t="n">
+      <c r="B27" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" s="17" t="n">
         <v>-60</v>
       </c>
-      <c r="D24" s="25" t="n">
+      <c r="D27" s="26" t="n">
         <v>3</v>
       </c>
-      <c r="E24" s="17" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1"/>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1"/>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1"/>
+      <c r="E27" s="17" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1"/>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1"/>
+    <row r="29" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1"/>
+      <c r="A30" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="0"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1"/>
+      <c r="A31" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="0"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1"/>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1"/>
+    <row r="33" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D33" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="E33" s="17" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1"/>
+      <c r="A34" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C34" s="17" t="n">
+        <v>-78</v>
+      </c>
+      <c r="D34" s="23" t="n">
+        <v>1</v>
+      </c>
+      <c r="E34" s="17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="17" t="n">
+        <v>2</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C35" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D35" s="17"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="27"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="17" t="n">
+        <v>3</v>
+      </c>
+      <c r="B36" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C36" s="17" t="n">
+        <v>-80</v>
+      </c>
+      <c r="D36" s="26" t="n">
+        <v>3</v>
+      </c>
+      <c r="E36" s="17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="17" t="n">
+        <v>4</v>
+      </c>
+      <c r="B37" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C37" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D37" s="17"/>
+      <c r="E37" s="17"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="17" t="n">
+        <v>5</v>
+      </c>
+      <c r="B38" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C38" s="17" t="n">
+        <v>-79</v>
+      </c>
+      <c r="D38" s="24" t="n">
+        <v>2</v>
+      </c>
+      <c r="E38" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="F38" s="27"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="17" t="n">
+        <v>6</v>
+      </c>
+      <c r="B39" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C39" s="17" t="n">
+        <v>-86</v>
+      </c>
+      <c r="D39" s="25" t="n">
+        <v>4</v>
+      </c>
+      <c r="E39" s="17" t="s">
+        <v>31</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
documentation updates PCBs/CC1101_868MHz_RF_Modul_FUEL4EP and PCBs/CC1101_868MHz_UFL_RF_Modul_FUEL4EP, sketches/FreqTest_range_test_with_distant_beacon/README.md and sketches/Range_test_beacon/README.md
</commit_message>
<xml_diff>
--- a/AsksinPP_developments/PCBs/CC1101_868MHz_RF_Modul_FUEL4EP/Prototype_Validation/validation_results.xlsx
+++ b/AsksinPP_developments/PCBs/CC1101_868MHz_RF_Modul_FUEL4EP/Prototype_Validation/validation_results.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="42">
   <si>
     <t xml:space="preserve">1. Frequenzmessung am GD0 Pin</t>
   </si>
@@ -108,7 +108,7 @@
     <t xml:space="preserve">Die gemessenen RSSI Werte sind nur als grobe Indikation des Empfangspegels zu sehen. Sie schwanken in aufeinanderfolgenden Messungen und hängen auch von kleinen Veränderungen, z.B. Bewegungen, im Umfeld ab.</t>
   </si>
   <si>
-    <t xml:space="preserve">a) mit zwei Betondecken zwischen  Zentrale und Empfänger</t>
+    <t xml:space="preserve">a) mit zwei Betondecken zwischen  Zentrale und Prüfempfänger</t>
   </si>
   <si>
     <t xml:space="preserve">gemessen mit Frequenztest mit ‚active Ping’: RSSI Wert des Signals von der Zentrale  bei 868,3 MHz, siehe FreqTest_active_ping_serial_monitor_&lt;#index&gt;_Erdgeschoss.log</t>
@@ -140,13 +140,25 @@
     <t xml:space="preserve">eByte E07-900MM10S </t>
   </si>
   <si>
-    <t xml:space="preserve">b) mit drei Betondecken zwischen  Zentrale und Empfänger</t>
+    <t xml:space="preserve">b) mit drei Betondecken zwischen  Zentrale und Prüfempfänger</t>
   </si>
   <si>
     <t xml:space="preserve">gemessen mit Frequenztest mit ‚active Ping’: RSSI Wert des Signals von der Zentrale  bei 868,3 MHz, siehe FreqTest_active_ping_serial_monitor_&lt;#index&gt;_Keller.log</t>
   </si>
   <si>
     <t xml:space="preserve">die Module unter Test (Device under Test DUT) wurden an der gleichen Stelle im Keller  mit dem identischen Frequenztest-Skript vermessen. Die Zentrale ist drei  Stockwerke höher im Dachgeschoss. Dazwischen sind 3 Betondecken.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. RSSI Empfangspegel mit Funkbake ‚Range_test_beacon’ und Prüfempfänger ‚FreqTest_range_test_with_distant_beacon‘</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a) mit 1,5  Stockwerken Distanz zwischen Funkbake in Abschirmdose und Prüfempfänger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gemessen mit ’FreqTest_range_test_with_distant_beacon’: RSSI Wert des Signals von der Zentrale  bei 868,3 MHz, siehe ‚FreqTest_range_test_with_distant_beacon_with_metal_can_and_1.5_floors_serial_monitor_&lt;#index&gt;.log‘</t>
+  </si>
+  <si>
+    <t xml:space="preserve">die Module unter Test (Device under Test DUT) wurden an der gleichen Stelle im Dachgeschoss  mit dem identischen Frequenztest-Skript ’FreqTest_range_test_with_distant_beacon’ vermessen. Die Funkbake ‚Range_test_beacon’  war 1,5 Stockwerke tiefer im Treppenhaus. Die Funkbake war zustätzlich mit einer Metalldose abgeschirmt.</t>
   </si>
 </sst>
 </file>
@@ -483,10 +495,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:O39"/>
+  <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I22" activeCellId="0" sqref="I22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F54" activeCellId="0" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1181,10 +1193,10 @@
         <v>22</v>
       </c>
       <c r="C38" s="17" t="n">
-        <v>-79</v>
-      </c>
-      <c r="D38" s="24" t="n">
-        <v>2</v>
+        <v>-86</v>
+      </c>
+      <c r="D38" s="25" t="n">
+        <v>4</v>
       </c>
       <c r="E38" s="17" t="s">
         <v>31</v>
@@ -1199,12 +1211,160 @@
         <v>34</v>
       </c>
       <c r="C39" s="17" t="n">
-        <v>-86</v>
-      </c>
-      <c r="D39" s="25" t="n">
+        <v>-79</v>
+      </c>
+      <c r="D39" s="24" t="n">
+        <v>2</v>
+      </c>
+      <c r="E39" s="17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="0"/>
+    </row>
+    <row r="43" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B43" s="3"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="0"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="0"/>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="0"/>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1"/>
+    </row>
+    <row r="47" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B47" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E39" s="17" t="s">
+      <c r="C47" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D47" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="E47" s="17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="B48" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C48" s="17" t="n">
+        <v>-100</v>
+      </c>
+      <c r="D48" s="26" t="n">
+        <v>3</v>
+      </c>
+      <c r="E48" s="17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="17" t="n">
+        <v>2</v>
+      </c>
+      <c r="B49" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C49" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D49" s="17"/>
+      <c r="E49" s="17"/>
+      <c r="F49" s="27"/>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="17" t="n">
+        <v>3</v>
+      </c>
+      <c r="B50" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C50" s="17" t="n">
+        <v>-99</v>
+      </c>
+      <c r="D50" s="24" t="n">
+        <v>2</v>
+      </c>
+      <c r="E50" s="17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="17" t="n">
+        <v>4</v>
+      </c>
+      <c r="B51" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C51" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D51" s="17"/>
+      <c r="E51" s="17"/>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="17" t="n">
+        <v>5</v>
+      </c>
+      <c r="B52" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C52" s="17" t="n">
+        <v>-104</v>
+      </c>
+      <c r="D52" s="25" t="n">
+        <v>4</v>
+      </c>
+      <c r="E52" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="F52" s="27"/>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="17" t="n">
+        <v>6</v>
+      </c>
+      <c r="B53" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C53" s="17" t="n">
+        <v>-97</v>
+      </c>
+      <c r="D53" s="23" t="n">
+        <v>1</v>
+      </c>
+      <c r="E53" s="17" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>